<commit_message>
Delete PatientID from Appointment table in Dev Doc and Project Doc. Add my hours to Final Checklist. Change name of Project Doc (spelling mistake)
</commit_message>
<xml_diff>
--- a/Final/DeveloperDocument.xlsx
+++ b/Final/DeveloperDocument.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28315"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baodinh/Desktop/INFO340/info340-final-project/Final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyleporter/Desktop/info340-final-project/Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15560" yWindow="820" windowWidth="18040" windowHeight="18740"/>
+    <workbookView xWindow="3340" yWindow="460" windowWidth="22260" windowHeight="14160"/>
   </bookViews>
   <sheets>
     <sheet name="Database Design" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="137">
   <si>
     <t>Patient Appointments Project</t>
   </si>
@@ -552,10 +552,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -872,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F154"/>
+  <dimension ref="A1:F150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -888,22 +888,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1264,16 +1264,16 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D24" t="s">
         <v>84</v>
       </c>
       <c r="F24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1281,7 +1281,7 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -1290,7 +1290,7 @@
         <v>84</v>
       </c>
       <c r="F25" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1298,68 +1298,68 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
         <v>9</v>
       </c>
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="3"/>
+      <c r="C28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="F29" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1367,16 +1367,16 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
         <v>71</v>
       </c>
       <c r="F30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1384,16 +1384,16 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
         <v>71</v>
       </c>
       <c r="F31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1401,16 +1401,16 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
         <v>33</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="F32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1418,7 +1418,7 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
         <v>33</v>
@@ -1427,7 +1427,7 @@
         <v>22</v>
       </c>
       <c r="F33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1435,16 +1435,16 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D34" t="s">
         <v>22</v>
       </c>
       <c r="F34" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1452,68 +1452,68 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
         <v>22</v>
       </c>
       <c r="F35" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" t="s">
-        <v>22</v>
-      </c>
-      <c r="F36" t="s">
-        <v>79</v>
-      </c>
+      <c r="A36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" s="3"/>
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="F38" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1521,7 +1521,7 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
@@ -1530,59 +1530,59 @@
         <v>84</v>
       </c>
       <c r="F39" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="A40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" t="s">
         <v>8</v>
       </c>
-      <c r="D40" t="s">
-        <v>84</v>
-      </c>
-      <c r="F40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" s="3"/>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="F42" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1590,7 +1590,7 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
@@ -1599,44 +1599,44 @@
         <v>84</v>
       </c>
       <c r="F43" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="A44" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" t="s">
         <v>8</v>
       </c>
-      <c r="D44" t="s">
-        <v>84</v>
-      </c>
-      <c r="F44" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>16</v>
+      <c r="D45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1644,16 +1644,16 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D46" t="s">
         <v>27</v>
       </c>
       <c r="F46" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1661,7 +1661,7 @@
         <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C47" t="s">
         <v>33</v>
@@ -1670,7 +1670,7 @@
         <v>27</v>
       </c>
       <c r="F47" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1678,16 +1678,16 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D48" t="s">
         <v>27</v>
       </c>
       <c r="F48" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1695,16 +1695,16 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C49" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D49" t="s">
         <v>27</v>
       </c>
       <c r="F49" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1712,7 +1712,7 @@
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C50" t="s">
         <v>33</v>
@@ -1721,7 +1721,7 @@
         <v>27</v>
       </c>
       <c r="F50" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1729,7 +1729,7 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C51" t="s">
         <v>33</v>
@@ -1738,7 +1738,7 @@
         <v>27</v>
       </c>
       <c r="F51" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1746,16 +1746,16 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D52" t="s">
         <v>27</v>
       </c>
       <c r="F52" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1763,68 +1763,68 @@
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C53" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D53" t="s">
         <v>27</v>
       </c>
       <c r="F53" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>7</v>
-      </c>
-      <c r="B54" t="s">
-        <v>44</v>
-      </c>
-      <c r="C54" t="s">
-        <v>46</v>
-      </c>
-      <c r="D54" t="s">
-        <v>27</v>
-      </c>
-      <c r="F54" t="s">
-        <v>114</v>
-      </c>
+      <c r="A54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F55" s="3"/>
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" t="s">
+        <v>27</v>
+      </c>
+      <c r="F55" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D56" t="s">
         <v>27</v>
       </c>
       <c r="F56" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -1832,7 +1832,7 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C57" t="s">
         <v>33</v>
@@ -1841,7 +1841,7 @@
         <v>27</v>
       </c>
       <c r="F57" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -1849,16 +1849,16 @@
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C58" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D58" t="s">
         <v>27</v>
       </c>
       <c r="F58" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -1866,68 +1866,68 @@
         <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D59" t="s">
         <v>27</v>
       </c>
       <c r="F59" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>7</v>
-      </c>
-      <c r="B60" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" t="s">
-        <v>33</v>
-      </c>
-      <c r="D60" t="s">
-        <v>27</v>
-      </c>
-      <c r="F60" t="s">
-        <v>99</v>
-      </c>
+      <c r="A60" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F60" s="3"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F61" s="3"/>
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61" t="s">
+        <v>27</v>
+      </c>
+      <c r="F61" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>7</v>
       </c>
       <c r="B62" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D62" t="s">
         <v>27</v>
       </c>
       <c r="F62" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -1935,16 +1935,16 @@
         <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D63" t="s">
         <v>27</v>
       </c>
       <c r="F63" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -1952,85 +1952,85 @@
         <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D64" t="s">
         <v>27</v>
       </c>
       <c r="F64" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>7</v>
-      </c>
-      <c r="B65" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65" t="s">
-        <v>8</v>
-      </c>
-      <c r="D65" t="s">
-        <v>27</v>
-      </c>
-      <c r="F65" t="s">
-        <v>105</v>
-      </c>
+      <c r="A65" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F65" s="3"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>7</v>
       </c>
       <c r="B66" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D66" t="s">
         <v>27</v>
       </c>
       <c r="F66" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F67" s="3"/>
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" t="s">
+        <v>27</v>
+      </c>
+      <c r="F67" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C68" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D68" t="s">
         <v>27</v>
       </c>
       <c r="F68" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -2038,7 +2038,7 @@
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="C69" t="s">
         <v>33</v>
@@ -2047,7 +2047,7 @@
         <v>27</v>
       </c>
       <c r="F69" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2055,16 +2055,16 @@
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="C70" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D70" t="s">
         <v>27</v>
       </c>
       <c r="F70" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2072,7 +2072,7 @@
         <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="C71" t="s">
         <v>33</v>
@@ -2081,7 +2081,7 @@
         <v>27</v>
       </c>
       <c r="F71" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2089,16 +2089,16 @@
         <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D72" t="s">
         <v>27</v>
       </c>
       <c r="F72" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2106,76 +2106,76 @@
         <v>7</v>
       </c>
       <c r="B73" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C73" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D73" t="s">
         <v>27</v>
       </c>
       <c r="F73" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>7</v>
-      </c>
-      <c r="B74" t="s">
-        <v>13</v>
-      </c>
-      <c r="C74" t="s">
-        <v>45</v>
-      </c>
-      <c r="D74" t="s">
-        <v>27</v>
-      </c>
-      <c r="F74" t="s">
-        <v>122</v>
-      </c>
+      <c r="A74" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F74" s="3"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="C75" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="D75" t="s">
         <v>27</v>
       </c>
       <c r="F75" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F76" s="3"/>
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" t="s">
+        <v>27</v>
+      </c>
+      <c r="F76" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="C77" t="s">
         <v>8</v>
@@ -2184,32 +2184,33 @@
         <v>27</v>
       </c>
       <c r="F77" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>7</v>
-      </c>
-      <c r="B78" t="s">
-        <v>36</v>
-      </c>
-      <c r="C78" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" t="s">
-        <v>27</v>
-      </c>
-      <c r="F78" t="s">
-        <v>106</v>
-      </c>
+      <c r="A78" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F78" s="3"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="C79" t="s">
         <v>8</v>
@@ -2218,33 +2219,32 @@
         <v>27</v>
       </c>
       <c r="F79" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F80" s="3"/>
+      <c r="A80" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80" t="s">
+        <v>55</v>
+      </c>
+      <c r="C80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" t="s">
+        <v>27</v>
+      </c>
+      <c r="F80" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>7</v>
       </c>
       <c r="B81" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="C81" t="s">
         <v>8</v>
@@ -2253,61 +2253,58 @@
         <v>27</v>
       </c>
       <c r="F81" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>7</v>
-      </c>
-      <c r="B82" t="s">
-        <v>55</v>
-      </c>
-      <c r="C82" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" t="s">
+        <v>36</v>
+      </c>
+      <c r="C84" t="s">
         <v>8</v>
       </c>
-      <c r="D82" t="s">
-        <v>27</v>
-      </c>
-      <c r="F82" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>7</v>
-      </c>
-      <c r="B83" t="s">
-        <v>9</v>
-      </c>
-      <c r="C83" t="s">
-        <v>8</v>
-      </c>
-      <c r="D83" t="s">
-        <v>27</v>
-      </c>
-      <c r="F83" t="s">
-        <v>116</v>
+      <c r="D84" t="s">
+        <v>29</v>
+      </c>
+      <c r="F84" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>16</v>
+      <c r="A85" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" t="s">
+        <v>37</v>
+      </c>
+      <c r="C85" t="s">
+        <v>33</v>
+      </c>
+      <c r="D85" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -2315,16 +2312,13 @@
         <v>23</v>
       </c>
       <c r="B86" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C86" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D86" t="s">
-        <v>29</v>
-      </c>
-      <c r="F86" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -2332,10 +2326,10 @@
         <v>23</v>
       </c>
       <c r="B87" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C87" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D87" t="s">
         <v>30</v>
@@ -2346,7 +2340,7 @@
         <v>23</v>
       </c>
       <c r="B88" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C88" t="s">
         <v>33</v>
@@ -2360,10 +2354,10 @@
         <v>23</v>
       </c>
       <c r="B89" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C89" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D89" t="s">
         <v>30</v>
@@ -2374,7 +2368,7 @@
         <v>23</v>
       </c>
       <c r="B90" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C90" t="s">
         <v>33</v>
@@ -2388,10 +2382,10 @@
         <v>23</v>
       </c>
       <c r="B91" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C91" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D91" t="s">
         <v>30</v>
@@ -2402,27 +2396,33 @@
         <v>23</v>
       </c>
       <c r="B92" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C92" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D92" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>23</v>
-      </c>
-      <c r="B93" t="s">
-        <v>43</v>
-      </c>
-      <c r="C93" t="s">
-        <v>45</v>
-      </c>
-      <c r="D93" t="s">
-        <v>30</v>
+      <c r="A93" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -2430,33 +2430,30 @@
         <v>23</v>
       </c>
       <c r="B94" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C94" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="D94" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="F94" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>16</v>
+      <c r="A95" t="s">
+        <v>23</v>
+      </c>
+      <c r="B95" t="s">
+        <v>37</v>
+      </c>
+      <c r="C95" t="s">
+        <v>33</v>
+      </c>
+      <c r="D95" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -2464,16 +2461,13 @@
         <v>23</v>
       </c>
       <c r="B96" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D96" t="s">
-        <v>29</v>
-      </c>
-      <c r="F96" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -2481,10 +2475,10 @@
         <v>23</v>
       </c>
       <c r="B97" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C97" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D97" t="s">
         <v>30</v>
@@ -2495,7 +2489,7 @@
         <v>23</v>
       </c>
       <c r="B98" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C98" t="s">
         <v>33</v>
@@ -2509,10 +2503,10 @@
         <v>23</v>
       </c>
       <c r="B99" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C99" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D99" t="s">
         <v>30</v>
@@ -2523,7 +2517,7 @@
         <v>23</v>
       </c>
       <c r="B100" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C100" t="s">
         <v>33</v>
@@ -2537,10 +2531,10 @@
         <v>23</v>
       </c>
       <c r="B101" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C101" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D101" t="s">
         <v>30</v>
@@ -2551,27 +2545,33 @@
         <v>23</v>
       </c>
       <c r="B102" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C102" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D102" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>23</v>
-      </c>
-      <c r="B103" t="s">
-        <v>43</v>
-      </c>
-      <c r="C103" t="s">
-        <v>45</v>
-      </c>
-      <c r="D103" t="s">
-        <v>30</v>
+      <c r="A103" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -2579,13 +2579,16 @@
         <v>23</v>
       </c>
       <c r="B104" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C104" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="D104" t="s">
-        <v>30</v>
+        <v>127</v>
+      </c>
+      <c r="F104" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -2593,7 +2596,7 @@
         <v>17</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>5</v>
@@ -2613,36 +2616,30 @@
         <v>23</v>
       </c>
       <c r="B106" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C106" t="s">
         <v>8</v>
       </c>
       <c r="D106" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="F106" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F107" s="3" t="s">
-        <v>16</v>
+      <c r="A107" t="s">
+        <v>23</v>
+      </c>
+      <c r="B107" t="s">
+        <v>56</v>
+      </c>
+      <c r="C107" t="s">
+        <v>33</v>
+      </c>
+      <c r="D107" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -2650,16 +2647,13 @@
         <v>23</v>
       </c>
       <c r="B108" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C108" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D108" t="s">
-        <v>29</v>
-      </c>
-      <c r="F108" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -2667,10 +2661,10 @@
         <v>23</v>
       </c>
       <c r="B109" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C109" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D109" t="s">
         <v>22</v>
@@ -2681,7 +2675,7 @@
         <v>23</v>
       </c>
       <c r="B110" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C110" t="s">
         <v>33</v>
@@ -2691,17 +2685,23 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>23</v>
-      </c>
-      <c r="B111" t="s">
-        <v>58</v>
-      </c>
-      <c r="C111" t="s">
-        <v>65</v>
-      </c>
-      <c r="D111" t="s">
-        <v>22</v>
+      <c r="A111" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -2709,33 +2709,30 @@
         <v>23</v>
       </c>
       <c r="B112" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C112" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D112" t="s">
+        <v>29</v>
+      </c>
+      <c r="F112" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>23</v>
+      </c>
+      <c r="B113" t="s">
+        <v>56</v>
+      </c>
+      <c r="C113" t="s">
+        <v>33</v>
+      </c>
+      <c r="D113" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -2743,16 +2740,13 @@
         <v>23</v>
       </c>
       <c r="B114" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C114" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D114" t="s">
-        <v>29</v>
-      </c>
-      <c r="F114" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -2760,10 +2754,10 @@
         <v>23</v>
       </c>
       <c r="B115" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C115" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D115" t="s">
         <v>22</v>
@@ -2774,7 +2768,7 @@
         <v>23</v>
       </c>
       <c r="B116" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C116" t="s">
         <v>33</v>
@@ -2784,17 +2778,23 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>23</v>
-      </c>
-      <c r="B117" t="s">
-        <v>58</v>
-      </c>
-      <c r="C117" t="s">
-        <v>65</v>
-      </c>
-      <c r="D117" t="s">
-        <v>22</v>
+      <c r="A117" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -2802,13 +2802,16 @@
         <v>23</v>
       </c>
       <c r="B118" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C118" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D118" t="s">
-        <v>22</v>
+        <v>127</v>
+      </c>
+      <c r="F118" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -2816,7 +2819,7 @@
         <v>17</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>5</v>
@@ -2836,36 +2839,30 @@
         <v>23</v>
       </c>
       <c r="B120" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C120" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D120" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="F120" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F121" s="3" t="s">
-        <v>16</v>
+      <c r="A121" t="s">
+        <v>23</v>
+      </c>
+      <c r="B121" t="s">
+        <v>55</v>
+      </c>
+      <c r="C121" t="s">
+        <v>8</v>
+      </c>
+      <c r="D121" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -2873,16 +2870,13 @@
         <v>23</v>
       </c>
       <c r="B122" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="C122" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D122" t="s">
-        <v>29</v>
-      </c>
-      <c r="F122" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -2890,27 +2884,33 @@
         <v>23</v>
       </c>
       <c r="B123" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="C123" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="D123" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>23</v>
-      </c>
-      <c r="B124" t="s">
-        <v>55</v>
-      </c>
-      <c r="C124" t="s">
-        <v>8</v>
-      </c>
-      <c r="D124" t="s">
-        <v>30</v>
+      <c r="A124" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -2918,13 +2918,16 @@
         <v>23</v>
       </c>
       <c r="B125" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C125" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="D125" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="F125" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
@@ -2932,33 +2935,27 @@
         <v>23</v>
       </c>
       <c r="B126" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C126" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="D126" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A127" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E127" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F127" s="3" t="s">
-        <v>16</v>
+      <c r="A127" t="s">
+        <v>23</v>
+      </c>
+      <c r="B127" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127" t="s">
+        <v>8</v>
+      </c>
+      <c r="D127" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
@@ -2966,30 +2963,33 @@
         <v>23</v>
       </c>
       <c r="B128" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C128" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="D128" t="s">
-        <v>29</v>
-      </c>
-      <c r="F128" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>23</v>
-      </c>
-      <c r="B129" t="s">
-        <v>36</v>
-      </c>
-      <c r="C129" t="s">
-        <v>70</v>
-      </c>
-      <c r="D129" t="s">
-        <v>30</v>
+      <c r="A129" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
@@ -2997,27 +2997,36 @@
         <v>23</v>
       </c>
       <c r="B130" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C130" t="s">
         <v>8</v>
       </c>
       <c r="D130" t="s">
-        <v>30</v>
+        <v>127</v>
+      </c>
+      <c r="F130" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>23</v>
-      </c>
-      <c r="B131" t="s">
-        <v>9</v>
-      </c>
-      <c r="C131" t="s">
-        <v>8</v>
-      </c>
-      <c r="D131" t="s">
-        <v>30</v>
+      <c r="A131" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
@@ -3025,33 +3034,30 @@
         <v>23</v>
       </c>
       <c r="B132" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="C132" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D132" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="F132" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A133" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E133" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F133" s="3" t="s">
-        <v>16</v>
+      <c r="A133" t="s">
+        <v>23</v>
+      </c>
+      <c r="B133" t="s">
+        <v>10</v>
+      </c>
+      <c r="C133" t="s">
+        <v>33</v>
+      </c>
+      <c r="D133" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
@@ -3059,36 +3065,27 @@
         <v>23</v>
       </c>
       <c r="B134" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C134" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="D134" t="s">
-        <v>127</v>
-      </c>
-      <c r="F134" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A135" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E135" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F135" s="3" t="s">
-        <v>16</v>
+      <c r="A135" t="s">
+        <v>23</v>
+      </c>
+      <c r="B135" t="s">
+        <v>64</v>
+      </c>
+      <c r="C135" t="s">
+        <v>33</v>
+      </c>
+      <c r="D135" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
@@ -3096,16 +3093,13 @@
         <v>23</v>
       </c>
       <c r="B136" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C136" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="D136" t="s">
-        <v>29</v>
-      </c>
-      <c r="F136" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
@@ -3113,7 +3107,7 @@
         <v>23</v>
       </c>
       <c r="B137" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C137" t="s">
         <v>33</v>
@@ -3127,10 +3121,10 @@
         <v>23</v>
       </c>
       <c r="B138" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C138" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D138" t="s">
         <v>30</v>
@@ -3141,27 +3135,33 @@
         <v>23</v>
       </c>
       <c r="B139" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C139" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D139" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>23</v>
-      </c>
-      <c r="B140" t="s">
-        <v>11</v>
-      </c>
-      <c r="C140" t="s">
-        <v>33</v>
-      </c>
-      <c r="D140" t="s">
-        <v>30</v>
+      <c r="A140" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
@@ -3169,13 +3169,16 @@
         <v>23</v>
       </c>
       <c r="B141" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C141" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="D141" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="F141" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
@@ -3183,10 +3186,10 @@
         <v>23</v>
       </c>
       <c r="B142" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C142" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D142" t="s">
         <v>30</v>
@@ -3197,33 +3200,27 @@
         <v>23</v>
       </c>
       <c r="B143" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C143" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="D143" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A144" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E144" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F144" s="3" t="s">
-        <v>16</v>
+      <c r="A144" t="s">
+        <v>23</v>
+      </c>
+      <c r="B144" t="s">
+        <v>64</v>
+      </c>
+      <c r="C144" t="s">
+        <v>33</v>
+      </c>
+      <c r="D144" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
@@ -3231,16 +3228,13 @@
         <v>23</v>
       </c>
       <c r="B145" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C145" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="D145" t="s">
-        <v>29</v>
-      </c>
-      <c r="F145" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
@@ -3248,7 +3242,7 @@
         <v>23</v>
       </c>
       <c r="B146" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C146" t="s">
         <v>33</v>
@@ -3262,10 +3256,10 @@
         <v>23</v>
       </c>
       <c r="B147" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C147" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D147" t="s">
         <v>30</v>
@@ -3276,27 +3270,33 @@
         <v>23</v>
       </c>
       <c r="B148" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C148" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D148" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>23</v>
-      </c>
-      <c r="B149" t="s">
-        <v>11</v>
-      </c>
-      <c r="C149" t="s">
-        <v>33</v>
-      </c>
-      <c r="D149" t="s">
-        <v>30</v>
+      <c r="A149" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
@@ -3304,77 +3304,15 @@
         <v>23</v>
       </c>
       <c r="B150" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C150" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D150" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>23</v>
-      </c>
-      <c r="B151" t="s">
-        <v>13</v>
-      </c>
-      <c r="C151" t="s">
-        <v>45</v>
-      </c>
-      <c r="D151" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
-        <v>23</v>
-      </c>
-      <c r="B152" t="s">
-        <v>14</v>
-      </c>
-      <c r="C152" t="s">
-        <v>46</v>
-      </c>
-      <c r="D152" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A153" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D153" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E153" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F153" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
-        <v>23</v>
-      </c>
-      <c r="B154" t="s">
-        <v>9</v>
-      </c>
-      <c r="C154" t="s">
-        <v>8</v>
-      </c>
-      <c r="D154" t="s">
         <v>127</v>
       </c>
-      <c r="F154" t="s">
+      <c r="F150" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix row labels on Views in Excel Sheet
</commit_message>
<xml_diff>
--- a/Final/DeveloperDocument.xlsx
+++ b/Final/DeveloperDocument.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="138">
   <si>
     <t>Patient Appointments Project</t>
   </si>
@@ -441,6 +441,9 @@
   </si>
   <si>
     <t>pDelClinic</t>
+  </si>
+  <si>
+    <t>View</t>
   </si>
 </sst>
 </file>
@@ -872,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F150"/>
+  <dimension ref="A1:F149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1604,7 +1607,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>94</v>
@@ -1777,7 +1780,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>100</v>
@@ -1880,7 +1883,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>101</v>
@@ -1966,7 +1969,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>102</v>
@@ -2120,7 +2123,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>103</v>
@@ -2189,7 +2192,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>104</v>
@@ -2256,24 +2259,41 @@
         <v>116</v>
       </c>
     </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>16</v>
+      <c r="A83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" t="s">
+        <v>36</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" t="s">
+        <v>29</v>
+      </c>
+      <c r="F83" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -2281,16 +2301,13 @@
         <v>23</v>
       </c>
       <c r="B84" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C84" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D84" t="s">
-        <v>29</v>
-      </c>
-      <c r="F84" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2298,7 +2315,7 @@
         <v>23</v>
       </c>
       <c r="B85" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C85" t="s">
         <v>33</v>
@@ -2312,10 +2329,10 @@
         <v>23</v>
       </c>
       <c r="B86" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C86" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D86" t="s">
         <v>30</v>
@@ -2326,10 +2343,10 @@
         <v>23</v>
       </c>
       <c r="B87" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C87" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D87" t="s">
         <v>30</v>
@@ -2340,7 +2357,7 @@
         <v>23</v>
       </c>
       <c r="B88" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C88" t="s">
         <v>33</v>
@@ -2354,7 +2371,7 @@
         <v>23</v>
       </c>
       <c r="B89" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C89" t="s">
         <v>33</v>
@@ -2368,10 +2385,10 @@
         <v>23</v>
       </c>
       <c r="B90" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C90" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D90" t="s">
         <v>30</v>
@@ -2382,47 +2399,50 @@
         <v>23</v>
       </c>
       <c r="B91" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C91" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D91" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>23</v>
-      </c>
-      <c r="B92" t="s">
-        <v>44</v>
-      </c>
-      <c r="C92" t="s">
-        <v>46</v>
-      </c>
-      <c r="D92" t="s">
-        <v>30</v>
+      <c r="A92" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>16</v>
+      <c r="A93" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" t="s">
+        <v>36</v>
+      </c>
+      <c r="C93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" t="s">
+        <v>29</v>
+      </c>
+      <c r="F93" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -2430,16 +2450,13 @@
         <v>23</v>
       </c>
       <c r="B94" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C94" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D94" t="s">
-        <v>29</v>
-      </c>
-      <c r="F94" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -2447,7 +2464,7 @@
         <v>23</v>
       </c>
       <c r="B95" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C95" t="s">
         <v>33</v>
@@ -2461,10 +2478,10 @@
         <v>23</v>
       </c>
       <c r="B96" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C96" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D96" t="s">
         <v>30</v>
@@ -2475,10 +2492,10 @@
         <v>23</v>
       </c>
       <c r="B97" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C97" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D97" t="s">
         <v>30</v>
@@ -2489,7 +2506,7 @@
         <v>23</v>
       </c>
       <c r="B98" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C98" t="s">
         <v>33</v>
@@ -2503,7 +2520,7 @@
         <v>23</v>
       </c>
       <c r="B99" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C99" t="s">
         <v>33</v>
@@ -2517,10 +2534,10 @@
         <v>23</v>
       </c>
       <c r="B100" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C100" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D100" t="s">
         <v>30</v>
@@ -2531,84 +2548,87 @@
         <v>23</v>
       </c>
       <c r="B101" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C101" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D101" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>23</v>
-      </c>
-      <c r="B102" t="s">
-        <v>44</v>
-      </c>
-      <c r="C102" t="s">
-        <v>46</v>
-      </c>
-      <c r="D102" t="s">
-        <v>30</v>
+      <c r="A102" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
+      <c r="A103" t="s">
+        <v>23</v>
+      </c>
+      <c r="B103" t="s">
+        <v>36</v>
+      </c>
+      <c r="C103" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" t="s">
+        <v>127</v>
+      </c>
+      <c r="F103" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B103" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C103" s="3" t="s">
+      <c r="B104" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C104" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D103" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E103" s="3" t="s">
+      <c r="D104" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E104" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F103" s="3" t="s">
+      <c r="F104" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>23</v>
-      </c>
-      <c r="B104" t="s">
-        <v>36</v>
-      </c>
-      <c r="C104" t="s">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>23</v>
+      </c>
+      <c r="B105" t="s">
+        <v>55</v>
+      </c>
+      <c r="C105" t="s">
         <v>8</v>
       </c>
-      <c r="D104" t="s">
-        <v>127</v>
-      </c>
-      <c r="F104" t="s">
+      <c r="D105" t="s">
+        <v>29</v>
+      </c>
+      <c r="F105" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -2616,16 +2636,13 @@
         <v>23</v>
       </c>
       <c r="B106" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C106" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D106" t="s">
-        <v>29</v>
-      </c>
-      <c r="F106" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -2633,7 +2650,7 @@
         <v>23</v>
       </c>
       <c r="B107" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C107" t="s">
         <v>33</v>
@@ -2647,10 +2664,10 @@
         <v>23</v>
       </c>
       <c r="B108" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C108" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D108" t="s">
         <v>22</v>
@@ -2661,47 +2678,50 @@
         <v>23</v>
       </c>
       <c r="B109" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C109" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D109" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>23</v>
-      </c>
-      <c r="B110" t="s">
-        <v>59</v>
-      </c>
-      <c r="C110" t="s">
-        <v>33</v>
-      </c>
-      <c r="D110" t="s">
-        <v>22</v>
+      <c r="A110" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>16</v>
+      <c r="A111" t="s">
+        <v>23</v>
+      </c>
+      <c r="B111" t="s">
+        <v>55</v>
+      </c>
+      <c r="C111" t="s">
+        <v>8</v>
+      </c>
+      <c r="D111" t="s">
+        <v>29</v>
+      </c>
+      <c r="F111" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -2709,16 +2729,13 @@
         <v>23</v>
       </c>
       <c r="B112" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C112" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D112" t="s">
-        <v>29</v>
-      </c>
-      <c r="F112" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -2726,7 +2743,7 @@
         <v>23</v>
       </c>
       <c r="B113" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C113" t="s">
         <v>33</v>
@@ -2740,10 +2757,10 @@
         <v>23</v>
       </c>
       <c r="B114" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C114" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D114" t="s">
         <v>22</v>
@@ -2754,84 +2771,87 @@
         <v>23</v>
       </c>
       <c r="B115" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C115" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D115" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>23</v>
-      </c>
-      <c r="B116" t="s">
-        <v>59</v>
-      </c>
-      <c r="C116" t="s">
-        <v>33</v>
-      </c>
-      <c r="D116" t="s">
-        <v>22</v>
+      <c r="A116" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="3" t="s">
+      <c r="A117" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" t="s">
+        <v>55</v>
+      </c>
+      <c r="C117" t="s">
+        <v>8</v>
+      </c>
+      <c r="D117" t="s">
+        <v>127</v>
+      </c>
+      <c r="F117" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B117" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C117" s="3" t="s">
+      <c r="B118" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C118" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D117" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E117" s="3" t="s">
+      <c r="D118" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E118" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F117" s="3" t="s">
+      <c r="F118" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>23</v>
-      </c>
-      <c r="B118" t="s">
-        <v>55</v>
-      </c>
-      <c r="C118" t="s">
-        <v>8</v>
-      </c>
-      <c r="D118" t="s">
-        <v>127</v>
-      </c>
-      <c r="F118" t="s">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>23</v>
+      </c>
+      <c r="B119" t="s">
+        <v>61</v>
+      </c>
+      <c r="C119" t="s">
+        <v>70</v>
+      </c>
+      <c r="D119" t="s">
+        <v>29</v>
+      </c>
+      <c r="F119" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F119" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -2839,16 +2859,13 @@
         <v>23</v>
       </c>
       <c r="B120" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C120" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D120" t="s">
-        <v>29</v>
-      </c>
-      <c r="F120" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -2856,7 +2873,7 @@
         <v>23</v>
       </c>
       <c r="B121" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C121" t="s">
         <v>8</v>
@@ -2870,47 +2887,50 @@
         <v>23</v>
       </c>
       <c r="B122" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="C122" t="s">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="D122" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>23</v>
-      </c>
-      <c r="B123" t="s">
-        <v>82</v>
-      </c>
-      <c r="C123" t="s">
-        <v>83</v>
-      </c>
-      <c r="D123" t="s">
-        <v>30</v>
+      <c r="A123" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F124" s="3" t="s">
-        <v>16</v>
+      <c r="A124" t="s">
+        <v>23</v>
+      </c>
+      <c r="B124" t="s">
+        <v>61</v>
+      </c>
+      <c r="C124" t="s">
+        <v>70</v>
+      </c>
+      <c r="D124" t="s">
+        <v>29</v>
+      </c>
+      <c r="F124" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -2918,16 +2938,13 @@
         <v>23</v>
       </c>
       <c r="B125" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C125" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D125" t="s">
-        <v>29</v>
-      </c>
-      <c r="F125" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
@@ -2935,7 +2952,7 @@
         <v>23</v>
       </c>
       <c r="B126" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C126" t="s">
         <v>8</v>
@@ -2949,84 +2966,87 @@
         <v>23</v>
       </c>
       <c r="B127" t="s">
+        <v>82</v>
+      </c>
+      <c r="C127" t="s">
+        <v>83</v>
+      </c>
+      <c r="D127" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>23</v>
+      </c>
+      <c r="B129" t="s">
+        <v>61</v>
+      </c>
+      <c r="C129" t="s">
+        <v>8</v>
+      </c>
+      <c r="D129" t="s">
+        <v>127</v>
+      </c>
+      <c r="F129" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>23</v>
+      </c>
+      <c r="B131" t="s">
         <v>9</v>
       </c>
-      <c r="C127" t="s">
-        <v>8</v>
-      </c>
-      <c r="D127" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>23</v>
-      </c>
-      <c r="B128" t="s">
-        <v>82</v>
-      </c>
-      <c r="C128" t="s">
-        <v>83</v>
-      </c>
-      <c r="D128" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F129" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>23</v>
-      </c>
-      <c r="B130" t="s">
-        <v>61</v>
-      </c>
-      <c r="C130" t="s">
-        <v>8</v>
-      </c>
-      <c r="D130" t="s">
-        <v>127</v>
-      </c>
-      <c r="F130" t="s">
+      <c r="C131" t="s">
+        <v>70</v>
+      </c>
+      <c r="D131" t="s">
+        <v>29</v>
+      </c>
+      <c r="F131" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A131" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D131" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E131" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F131" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
@@ -3034,16 +3054,13 @@
         <v>23</v>
       </c>
       <c r="B132" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C132" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="D132" t="s">
-        <v>29</v>
-      </c>
-      <c r="F132" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
@@ -3051,10 +3068,10 @@
         <v>23</v>
       </c>
       <c r="B133" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="C133" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D133" t="s">
         <v>30</v>
@@ -3065,10 +3082,10 @@
         <v>23</v>
       </c>
       <c r="B134" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C134" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D134" t="s">
         <v>30</v>
@@ -3079,7 +3096,7 @@
         <v>23</v>
       </c>
       <c r="B135" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="C135" t="s">
         <v>33</v>
@@ -3093,7 +3110,7 @@
         <v>23</v>
       </c>
       <c r="B136" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C136" t="s">
         <v>33</v>
@@ -3107,10 +3124,10 @@
         <v>23</v>
       </c>
       <c r="B137" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C137" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D137" t="s">
         <v>30</v>
@@ -3121,47 +3138,50 @@
         <v>23</v>
       </c>
       <c r="B138" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C138" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D138" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>23</v>
-      </c>
-      <c r="B139" t="s">
-        <v>14</v>
-      </c>
-      <c r="C139" t="s">
-        <v>46</v>
-      </c>
-      <c r="D139" t="s">
-        <v>30</v>
+      <c r="A139" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A140" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D140" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E140" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F140" s="3" t="s">
-        <v>16</v>
+      <c r="A140" t="s">
+        <v>23</v>
+      </c>
+      <c r="B140" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140" t="s">
+        <v>70</v>
+      </c>
+      <c r="D140" t="s">
+        <v>29</v>
+      </c>
+      <c r="F140" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
@@ -3169,16 +3189,13 @@
         <v>23</v>
       </c>
       <c r="B141" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C141" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="D141" t="s">
-        <v>29</v>
-      </c>
-      <c r="F141" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
@@ -3186,10 +3203,10 @@
         <v>23</v>
       </c>
       <c r="B142" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="C142" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D142" t="s">
         <v>30</v>
@@ -3200,10 +3217,10 @@
         <v>23</v>
       </c>
       <c r="B143" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C143" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D143" t="s">
         <v>30</v>
@@ -3214,7 +3231,7 @@
         <v>23</v>
       </c>
       <c r="B144" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="C144" t="s">
         <v>33</v>
@@ -3228,7 +3245,7 @@
         <v>23</v>
       </c>
       <c r="B145" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C145" t="s">
         <v>33</v>
@@ -3242,10 +3259,10 @@
         <v>23</v>
       </c>
       <c r="B146" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C146" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D146" t="s">
         <v>30</v>
@@ -3256,63 +3273,49 @@
         <v>23</v>
       </c>
       <c r="B147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C147" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D147" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
-        <v>23</v>
-      </c>
-      <c r="B148" t="s">
-        <v>14</v>
-      </c>
-      <c r="C148" t="s">
-        <v>46</v>
-      </c>
-      <c r="D148" t="s">
-        <v>30</v>
+      <c r="A148" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F148" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A149" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F149" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
-        <v>23</v>
-      </c>
-      <c r="B150" t="s">
+      <c r="A149" t="s">
+        <v>23</v>
+      </c>
+      <c r="B149" t="s">
         <v>9</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C149" t="s">
         <v>8</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D149" t="s">
         <v>127</v>
       </c>
-      <c r="F150" t="s">
+      <c r="F149" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>